<commit_message>
Continuação dos Estudos sobre Excel Básico
</commit_message>
<xml_diff>
--- a/excel-basico/introducao.xlsx
+++ b/excel-basico/introducao.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiq98\Downloads\excel-curso\excel-basico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9464E6-C7A7-464B-8F56-147D6F23B016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E1C779-013B-4588-A677-18EB3A8EA360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Tópico</t>
   </si>
@@ -76,13 +78,124 @@
   </si>
   <si>
     <t>Ensina como alterar tipo, tamanho, cor e estilo da fonte (negrito, itálico, sublinhado) para melhorar a aparência dos dados.</t>
+  </si>
+  <si>
+    <t>Formatando números</t>
+  </si>
+  <si>
+    <t>Mostra como aplicar formatos como moeda, porcentagem, número com separador de milhar e casas decimais.</t>
+  </si>
+  <si>
+    <t>Formatando Datas</t>
+  </si>
+  <si>
+    <t>Explica como configurar diferentes formatos de data (ex: DD/MM/AAAA, abreviações, data longa, etc.).</t>
+  </si>
+  <si>
+    <t>Salvando arquivo do Excel</t>
+  </si>
+  <si>
+    <t>Orienta como salvar arquivos no formato XLSX, além de salvar como PDF ou com outro nome/pasta.</t>
+  </si>
+  <si>
+    <t>Renomear as planilhas</t>
+  </si>
+  <si>
+    <t>Mostra como alterar o nome das abas das planilhas para organização mais clara.</t>
+  </si>
+  <si>
+    <t>Mover, Ocultar e Reexibir Planilhas</t>
+  </si>
+  <si>
+    <t>Explica como reorganizar a ordem das planilhas, ocultá-las ou torná-las visíveis novamente.</t>
+  </si>
+  <si>
+    <t>Mudar cor da Guia</t>
+  </si>
+  <si>
+    <t>Ensina a aplicar cores nas abas das planilhas para facilitar a identificação visual.</t>
+  </si>
+  <si>
+    <t>Copiando e colando formatações</t>
+  </si>
+  <si>
+    <t>Demonstra como usar o Pincel de Formatação para replicar estilos de célula em outras partes da planilha.</t>
+  </si>
+  <si>
+    <t>Alinhar Linhas e Colunas</t>
+  </si>
+  <si>
+    <t>Explica como alinhar o conteúdo das células horizontal e verticalmente para melhor apresentação dos dados.</t>
+  </si>
+  <si>
+    <t>Inserindo Linhas e Colunas</t>
+  </si>
+  <si>
+    <t>Mostra como adicionar novas linhas ou colunas entre dados já existentes na planilha.</t>
+  </si>
+  <si>
+    <t>Deletando Linhas e Colunas</t>
+  </si>
+  <si>
+    <t>Ensina como excluir linhas ou colunas indesejadas sem afetar o restante da estrutura da planilha.</t>
+  </si>
+  <si>
+    <t>Desfazer e Refazer Mudanças na planilha</t>
+  </si>
+  <si>
+    <t>Demonstra como usar os comandos de desfazer (Ctrl + Z) e refazer (Ctrl + Y) para corrigir ações.</t>
+  </si>
+  <si>
+    <t>Mesclar Células</t>
+  </si>
+  <si>
+    <t>Explica como unir duas ou mais células em uma única, útil para títulos e formatações específicas.</t>
+  </si>
+  <si>
+    <t>Ocultar Linhas e Colunas</t>
+  </si>
+  <si>
+    <t>Mostra como ocultar partes da planilha sem excluir dados, útil para focar no que é relevante.</t>
+  </si>
+  <si>
+    <t>Re-Exibir Linhas e Colunas</t>
+  </si>
+  <si>
+    <t>Ensina como tornar visíveis novamente linhas ou colunas ocultas anteriormente.</t>
+  </si>
+  <si>
+    <t>Inserindo Formas</t>
+  </si>
+  <si>
+    <t>Apresenta como adicionar formas geométricas, setas ou elementos gráficos à planilha.</t>
+  </si>
+  <si>
+    <t>Adicionando Plano de Fundo</t>
+  </si>
+  <si>
+    <t>Mostra como inserir uma imagem ou cor de fundo na planilha para fins visuais ou personalizados.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="13">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="171" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="173" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="174" formatCode="[$-416]d\-mmm;@"/>
+    <numFmt numFmtId="175" formatCode="[$-416]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="176" formatCode="[$-409]d/m/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="177" formatCode="mmmm\,\ yyyy;@"/>
+    <numFmt numFmtId="178" formatCode="[$-416]d;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +206,13 @@
     <font>
       <b/>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -137,10 +257,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,11 +271,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -431,16 +573,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
     <col min="3" max="3" width="128.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -459,10 +601,10 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -470,10 +612,10 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -481,10 +623,10 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
     </row>
@@ -492,10 +634,10 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="18" t="s">
         <v>12</v>
       </c>
     </row>
@@ -503,10 +645,10 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -514,10 +656,10 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -525,10 +667,10 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -536,100 +678,320 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="4"/>
+      <c r="B21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAA85A1-68B3-4F52-BE4B-3C03D23AF083}">
+  <dimension ref="B2:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>-11000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0089019-71CE-4491-A630-79EF6DB74C56}">
+  <dimension ref="B5:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="13">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="14">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>54903</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="17">
+        <v>54903</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>